<commit_message>
test héritage fr-core-practitioner bc68d94b8e8160156cfccd7aca6012967defcecf
</commit_message>
<xml_diff>
--- a/sd-add-new-fr-core/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/sd-add-new-fr-core/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-03T17:09:56+00:00</t>
+    <t>2024-04-04T08:25:00+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -66,7 +66,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>ANS (https://esante.gouv.fr)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>